<commit_message>
Create arena page was updated. Creation was provided. Update arenas list in competition page was provided.
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="sportsman-page.html" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="competition-page.html" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="group-page.html" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="creating-pairs-list-page.html" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="499">
   <si>
     <t xml:space="preserve">origin</t>
   </si>
@@ -1384,6 +1385,144 @@
   </si>
   <si>
     <t xml:space="preserve">Додати спортсменів </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_PAGE_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create arena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Створити арену</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Создать арену</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_PLACE_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arena name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Назва арени</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Название арены</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_AUTOSORT_TAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatic sorting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Автоматичне сортування</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Автоматическая сортировка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_MANUAL_TAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual sorting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ручне сортування</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ручная сортировка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_ACTIVE_GROUPS_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selected groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Обрані групи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выбранные группы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_UNACTIVE_GROUPS_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groups list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Список груп</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Список групп</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_DISTANCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One member pairs distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Відстань між парами одного учасника</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Расстояние между парами одного участника</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_AGE_MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_AGE_MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_WEIGHT_MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_WEIGHT_MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_FINAL_MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_FINAL_MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_APPLY_BTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СТВОРИТИ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СОЗДАТЬ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_ACTIVE_PAIRS_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selected pairs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Обрані пари</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выбранные пары</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_UNACTIVE_PAIRS_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unattached pairs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Неприв’язані пари</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Непривязанные пары</t>
   </si>
 </sst>
 </file>
@@ -1393,7 +1532,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1415,12 +1554,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1465,16 +1598,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1501,8 +1630,8 @@
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H25:H26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1510,7 +1639,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
   </cols>
   <sheetData>
@@ -1655,7 +1784,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -1669,7 +1798,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -1683,7 +1812,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -1697,7 +1826,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B14" s="0" t="s">
@@ -1711,7 +1840,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B15" s="0" t="s">
@@ -1725,7 +1854,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B16" s="0" t="s">
@@ -1739,7 +1868,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="0" t="s">
@@ -1879,7 +2008,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B27" s="0" t="s">
@@ -1921,7 +2050,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B30" s="0" t="s">
@@ -1963,10 +2092,10 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C33" s="0" t="s">
@@ -1996,7 +2125,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="1" sqref="H25:H26 A19"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2024,7 +2153,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2038,7 +2167,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2052,7 +2181,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2066,7 +2195,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2080,7 +2209,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2094,7 +2223,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2136,7 +2265,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>157</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2234,7 +2363,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2248,7 +2377,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2262,7 +2391,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2374,7 +2503,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="1" sqref="H25:H26 D5"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2401,7 +2530,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>206</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -2475,7 +2604,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="H25:H26 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2530,7 +2659,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>219</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -2968,7 +3097,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="1" sqref="H25:H26 D36"/>
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3037,7 +3166,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>287</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -3541,7 +3670,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>366</v>
       </c>
       <c r="B41" s="0" t="s">
@@ -3586,8 +3715,8 @@
   </sheetPr>
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D44" activeCellId="1" sqref="H25:H26 D44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3617,7 +3746,7 @@
       <c r="A2" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>374</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -4090,7 +4219,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>432</v>
       </c>
       <c r="B36" s="0" t="s">
@@ -4199,6 +4328,275 @@
       </c>
       <c r="D43" s="0" t="s">
         <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H35" activeCellId="0" sqref="H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First preparation for arena page was provided: common names and links, tabs, pairs list
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <sheet name="competition-page.html" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="group-page.html" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="creating-pairs-list-page.html" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="location-page.html" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="525">
   <si>
     <t xml:space="preserve">origin</t>
   </si>
@@ -1523,6 +1524,84 @@
   </si>
   <si>
     <t xml:space="preserve">Непривязанные пары</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_PAIRS_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_SETTINGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Налаштування</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Настройки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_ROUND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_TIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_RED_SPORTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_BLUE_SPORTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_GROUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Група</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Группа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_WINNER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_RED_SCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Червоний рахунок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Красный счёт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_BLUE_SCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Синій рахунок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Синий счёт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_PAIR_WINNER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winner of pair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Переможець пари</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Победитель пары</t>
   </si>
 </sst>
 </file>
@@ -1631,7 +1710,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+      <selection pane="topLeft" activeCell="H26" activeCellId="1" sqref="A1:D12 H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2125,7 +2204,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="1" sqref="A1:D12 A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2503,7 +2582,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2604,7 +2683,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3097,7 +3176,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+      <selection pane="topLeft" activeCell="D36" activeCellId="1" sqref="A1:D12 D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3716,7 +3795,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4348,8 +4427,8 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H35" activeCellId="0" sqref="H35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4608,4 +4687,208 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="5" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>524</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added delete arena btn
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="537">
   <si>
     <t xml:space="preserve">origin</t>
   </si>
@@ -1602,6 +1602,42 @@
   </si>
   <si>
     <t xml:space="preserve">Победитель пары</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_REFRESH_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refresh the list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Оновити список</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Обновить список</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_START_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Старт списку</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Старт списка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_DELETE_ARENA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete arena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Видалити арена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Удалить арена</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1647,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1633,6 +1669,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1677,7 +1719,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1690,36 +1732,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="1" sqref="A1:D12 H26"/>
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2197,24 +2242,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="1" sqref="A1:D12 A19"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="14.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="14.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2575,23 +2620,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="A1:D12"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2676,23 +2720,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="A1:D12"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3169,23 +3212,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="1" sqref="A1:D12 D36"/>
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3788,23 +3830,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="A1:D12"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4421,23 +4462,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="A1:D12"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4690,28 +4730,26 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D12"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="5" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4880,6 +4918,48 @@
       </c>
       <c r="D12" s="0" t="s">
         <v>524</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>535</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add/delete pairs to arena operations were provided.
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="533">
   <si>
     <t xml:space="preserve">origin</t>
   </si>
@@ -1602,6 +1602,30 @@
   </si>
   <si>
     <t xml:space="preserve">Победитель пары</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_ADD_PAIRS_TO_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pairs adding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Додавання пар</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добавление пар</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHX_ADD_PAIRS_BTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Додати</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добавить</t>
   </si>
 </sst>
 </file>
@@ -1710,7 +1734,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="1" sqref="A1:D12 H26"/>
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2204,7 +2228,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="1" sqref="A1:D12 A19"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2582,7 +2606,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="A1:D12"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2683,7 +2707,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="A1:D12"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3176,7 +3200,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="1" sqref="A1:D12 D36"/>
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3795,7 +3819,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="A1:D12"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4428,7 +4452,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="A1:D12"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4694,24 +4718,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:D12"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="5" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="22.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4880,6 +4895,34 @@
       </c>
       <c r="D12" s="0" t="s">
         <v>524</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arena create page was updated: fixes for schedule
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
     <sheet name="sportsman-page.html" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="competition-page.html" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="group-page.html" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="creating-pairs-list-page.html" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="create-arena-page.html" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="location-page.html" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="540">
   <si>
     <t xml:space="preserve">origin</t>
   </si>
@@ -848,487 +848,496 @@
     <t xml:space="preserve">PH28_PAIR_LIST</t>
   </si>
   <si>
+    <t xml:space="preserve">Arena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Арена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH29_PAIR_TIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Час</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Время</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH30_PAIR_RES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH31_INFO_TRAINER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH32_INFO_REGION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH1_SPORTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH2_GROUPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH3_PAIRS_LISTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arenas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Арени</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Арены</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH4_INFO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH5_SORT_BTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update groups composition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Оновити склад груп</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Обновить состав групп</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH6_SPORTS_TBL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH7_SPORT_SURNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH8_SPORT_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH9_SPORT_AGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вік</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Возраст</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH10_SPORT_WEIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH11_SPORT_SEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH12_SPORT_TEAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH13_SPORT_QUAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH14_SPORT_ADMIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admitton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH15_SPORT_GR_NUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groups number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кількість груп</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Количество групп</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH16_GROUPS_TBL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH17_GROUP_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH18_GROUP_AGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH19_GROUP_SEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH20_GROUP_DISC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH21_GROUP_WEIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH22_GROUP_QUAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH23_GROUP_SP_NUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sportsmen number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кількість спортсменів</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Количество спортсменов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH24_ADD_PAIRS_LIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create pairs list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Створити список пар</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Создать список пар</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH25_INFO_HEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH26_INFO_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH27_INFO_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH28_INFO_DESC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH29_INFO_START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH30_INFO_END</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH31_SPORTS_ADD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sportsmen adding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Додавання спротсменів</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добавление спортсменов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH32_SPORTS_ADD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add sportsmen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дадати спортсменів</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добавить спортсменов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH33_GROUPS_ADD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group creation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Створення групи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Создание группы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH34_GROUP_SYSTEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Система</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH35_GROUP_AGE_MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimal age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мінімальний вік</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Минимальный возраст</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH36_GROUP_AGE_MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximal age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Максимальний вік</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Максимальный возраст</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH37_GROUP_WEIGHT_MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimal weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мінімальна вага</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Минимальный вес</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH38_GROUP_WEIGHT_MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximal weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Максимальна вага</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Максимальный вес</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH39_GROUP_QUAL_MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimal qualification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мінімальна кваліфікація</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Минимальная квалификация</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH40_GROUP_QUAL_MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximal qualification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Максимальна кваліфікація</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Максимальная квалификация</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH41_GROUP_CREATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Створити групу</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Создать группу</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH3_PAIRS_TAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH4_GRID_TAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сітка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сетка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH5_INFO_HEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH7_INFO_SYSTEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH8_INFO_DISCIPLINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH9_INFO_SEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH10_INFO_LOW_AGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH11_INFO_TOP_AGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH12_INFO_LOW_WEIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH13_INFO_TOP_WEIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH14_INFO_LOW_QUAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH15_INFO_TOP_QUAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH16_FORMULAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formulas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Формули</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Формулы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH17_PREPARATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preparation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Підготовка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Подготовка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH18_ROUNDS_NUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rounds number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кількість раундів</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Количество раундов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH19_ROUND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Round</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Раунд</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH20_REST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Відпочинок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Отдых</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH21_HOLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Затримка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Задержка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH22_FINAL_MIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimal final part</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мінімальна фінальна частина</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Минимальная финальная часть</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH23_FINAL_MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximal final part</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Максимальна фінальна частина</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Максимальная финальная часть</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH24_DELETE_BTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH25_SPORTS_TBL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH26_SPORT_SURNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH27_SPORT_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH28_SPORT_AGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH29_SPORT_WEIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH30_SPORT_SEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH31_SPORT_TEAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH32_SPORT_QUAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH33_SPORT_ADMIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH34_PAIRS_TBL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH35_PAIRS_NUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PH36_PAIRS_LIST</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pairs list</t>
   </si>
   <si>
     <t xml:space="preserve">Список пар</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH29_PAIR_TIME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Час</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Время</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH30_PAIR_RES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH31_INFO_TRAINER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH32_INFO_REGION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH1_SPORTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH2_GROUPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH3_PAIRS_LISTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pairs lists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Списки пар</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH4_INFO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH5_SORT_BTN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update groups composition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Оновити склад груп</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Обновить состав групп</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH6_SPORTS_TBL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH7_SPORT_SURNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH8_SPORT_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH9_SPORT_AGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Вік</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Возраст</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH10_SPORT_WEIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH11_SPORT_SEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH12_SPORT_TEAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH13_SPORT_QUAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH14_SPORT_ADMIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admitton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH15_SPORT_GR_NUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Groups number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кількість груп</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Количество групп</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH16_GROUPS_TBL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH17_GROUP_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH18_GROUP_AGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH19_GROUP_SEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH20_GROUP_DISC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH21_GROUP_WEIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH22_GROUP_QUAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH23_GROUP_SP_NUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sportsmen number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кількість спортсменів</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Количество спортсменов</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH24_ADD_PAIRS_LIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create pairs list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Створити список пар</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Создать список пар</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH25_INFO_HEAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH26_INFO_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH27_INFO_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH28_INFO_DESC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH29_INFO_START</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH30_INFO_END</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH31_SPORTS_ADD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sportsmen adding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Додавання спротсменів</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Добавление спортсменов</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH32_SPORTS_ADD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add sportsmen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дадати спортсменів</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Добавить спортсменов</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH33_GROUPS_ADD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group creation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Створення групи</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Создание группы</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH34_GROUP_SYSTEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Система</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH35_GROUP_AGE_MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimal age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Мінімальний вік</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Минимальный возраст</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH36_GROUP_AGE_MAX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximal age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Максимальний вік</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Максимальный возраст</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH37_GROUP_WEIGHT_MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimal weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Мінімальна вага</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Минимальный вес</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH38_GROUP_WEIGHT_MAX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximal weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Максимальна вага</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Максимальный вес</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH39_GROUP_QUAL_MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimal qualification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Мінімальна кваліфікація</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Минимальная квалификация</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH40_GROUP_QUAL_MAX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximal qualification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Максимальна кваліфікація</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Максимальная квалификация</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH41_GROUP_CREATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Створити групу</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Создать группу</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH3_PAIRS_TAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH4_GRID_TAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сітка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сетка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH5_INFO_HEAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH7_INFO_SYSTEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH8_INFO_DISCIPLINE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH9_INFO_SEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH10_INFO_LOW_AGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH11_INFO_TOP_AGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH12_INFO_LOW_WEIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH13_INFO_TOP_WEIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH14_INFO_LOW_QUAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH15_INFO_TOP_QUAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH16_FORMULAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formulas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Формули</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Формулы</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH17_PREPARATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preparation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Підготовка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Подготовка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH18_ROUNDS_NUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rounds number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кількість раундів</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Количество раундов</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH19_ROUND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Round</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Раунд</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH20_REST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Відпочинок</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Отдых</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH21_HOLD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Затримка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Задержка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH22_FINAL_MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimal final part</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Мінімальна фінальна частина</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Минимальная финальная часть</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH23_FINAL_MAX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximal final part</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Максимальна фінальна частина</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Максимальная финальная часть</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH24_DELETE_BTN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH25_SPORTS_TBL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH26_SPORT_SURNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH27_SPORT_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH28_SPORT_AGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH29_SPORT_WEIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH30_SPORT_SEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH31_SPORT_TEAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH32_SPORT_QUAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH33_SPORT_ADMIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH34_PAIRS_TBL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH35_PAIRS_NUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PH36_PAIRS_LIST</t>
   </si>
   <si>
     <t xml:space="preserve">PH37_PAIR_TIME</t>
@@ -1647,7 +1656,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1669,12 +1678,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1719,7 +1722,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1732,24 +1735,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1759,12 +1758,13 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,24 +2242,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="8.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="14.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="14.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,22 +2620,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2720,22 +2721,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3130,7 +3132,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>272</v>
       </c>
@@ -3212,22 +3214,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3283,12 +3286,12 @@
         <v>286</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>134</v>
@@ -3302,21 +3305,21 @@
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>130</v>
@@ -3330,7 +3333,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>45</v>
@@ -3344,7 +3347,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>41</v>
@@ -3358,21 +3361,21 @@
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>53</v>
@@ -3386,7 +3389,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>57</v>
@@ -3400,7 +3403,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>61</v>
@@ -3414,7 +3417,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>68</v>
@@ -3428,10 +3431,10 @@
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>257</v>
@@ -3442,21 +3445,21 @@
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>239</v>
@@ -3470,7 +3473,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>41</v>
@@ -3484,21 +3487,21 @@
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>57</v>
@@ -3512,7 +3515,7 @@
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>263</v>
@@ -3526,7 +3529,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>53</v>
@@ -3540,7 +3543,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>68</v>
@@ -3554,35 +3557,35 @@
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>134</v>
@@ -3596,7 +3599,7 @@
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>75</v>
@@ -3610,7 +3613,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>41</v>
@@ -3624,10 +3627,10 @@
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>179</v>
@@ -3638,7 +3641,7 @@
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>182</v>
@@ -3652,7 +3655,7 @@
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>186</v>
@@ -3666,156 +3669,156 @@
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -3830,7 +3833,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3840,12 +3843,13 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3867,7 +3871,7 @@
         <v>206</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>135</v>
@@ -3892,7 +3896,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>243</v>
@@ -3906,21 +3910,21 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>134</v>
@@ -3948,21 +3952,21 @@
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>263</v>
@@ -3976,7 +3980,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>57</v>
@@ -3990,203 +3994,203 @@
     </row>
     <row r="11" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>213</v>
@@ -4200,7 +4204,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>130</v>
@@ -4214,7 +4218,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>45</v>
@@ -4228,7 +4232,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>41</v>
@@ -4242,21 +4246,21 @@
     </row>
     <row r="29" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>53</v>
@@ -4270,7 +4274,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>57</v>
@@ -4284,7 +4288,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>61</v>
@@ -4298,7 +4302,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>68</v>
@@ -4312,7 +4316,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>256</v>
@@ -4326,7 +4330,7 @@
     </row>
     <row r="35" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>243</v>
@@ -4340,7 +4344,7 @@
     </row>
     <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>271</v>
@@ -4354,21 +4358,21 @@
     </row>
     <row r="37" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>273</v>
+        <v>435</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>274</v>
+        <v>436</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>274</v>
+        <v>436</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>276</v>
@@ -4382,72 +4386,72 @@
     </row>
     <row r="39" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -4462,22 +4466,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="9.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4496,226 +4501,226 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -4730,26 +4735,28 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="5" style="0" width="9.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="9.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4768,49 +4775,49 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>273</v>
+        <v>435</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>274</v>
+        <v>436</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>274</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>276</v>
@@ -4824,142 +4831,142 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>525</v>
+      <c r="A13" s="1" t="s">
+        <v>528</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>529</v>
+      <c r="A14" s="1" t="s">
+        <v>532</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>533</v>
+      <c r="A15" s="1" t="s">
+        <v>536</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arena page was renamed. Datetimepicker on department page was corrected
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
     <sheet name="competition-page.html" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="group-page.html" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="create-arena-page.html" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="location-page.html" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="arena-page.html" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -3220,7 +3220,7 @@
   </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -4741,7 +4741,7 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Date format was fixed. One more flag for sporsmen was fixed
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="541">
   <si>
     <t xml:space="preserve">origin</t>
   </si>
@@ -404,6 +404,18 @@
     <t xml:space="preserve">ВВЕДИТЕ НОВЫЙ ПАРОЛЬ СНОВА</t>
   </si>
   <si>
+    <t xml:space="preserve">CPH32_HUMAN_AGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вік</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Возраст</t>
+  </si>
+  <si>
     <t xml:space="preserve">PH1_COMP_TAB</t>
   </si>
   <si>
@@ -918,15 +930,6 @@
   </si>
   <si>
     <t xml:space="preserve">PH9_SPORT_AGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Вік</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Возраст</t>
   </si>
   <si>
     <t xml:space="preserve">PH10_SPORT_WEIGHT</t>
@@ -1754,11 +1757,11 @@
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.82"/>
@@ -2117,7 +2120,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>93</v>
       </c>
@@ -2173,7 +2176,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>109</v>
       </c>
@@ -2187,7 +2190,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>113</v>
       </c>
@@ -2229,7 +2232,20 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2278,310 +2294,310 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2655,21 +2671,21 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>61</v>
@@ -2683,30 +2699,30 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2756,49 +2772,49 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>75</v>
@@ -2812,7 +2828,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>45</v>
@@ -2826,7 +2842,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>41</v>
@@ -2840,7 +2856,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>57</v>
@@ -2854,7 +2870,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>49</v>
@@ -2868,7 +2884,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>53</v>
@@ -2882,7 +2898,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>68</v>
@@ -2896,7 +2912,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>61</v>
@@ -2910,287 +2926,287 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>64</v>
@@ -3249,91 +3265,91 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>45</v>
@@ -3347,7 +3363,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>41</v>
@@ -3361,21 +3377,21 @@
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>297</v>
+        <v>126</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>298</v>
+        <v>127</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>299</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>53</v>
@@ -3389,7 +3405,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>57</v>
@@ -3403,7 +3419,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>61</v>
@@ -3417,7 +3433,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>68</v>
@@ -3431,49 +3447,49 @@
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>41</v>
@@ -3487,21 +3503,21 @@
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>297</v>
+        <v>126</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>298</v>
+        <v>127</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>299</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>57</v>
@@ -3515,21 +3531,21 @@
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>53</v>
@@ -3543,7 +3559,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>68</v>
@@ -3557,49 +3573,49 @@
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>75</v>
@@ -3613,7 +3629,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>41</v>
@@ -3627,198 +3643,198 @@
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -3868,77 +3884,77 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>41</v>
@@ -3952,35 +3968,35 @@
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>57</v>
@@ -3994,231 +4010,231 @@
     </row>
     <row r="11" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>45</v>
@@ -4232,7 +4248,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>41</v>
@@ -4246,21 +4262,21 @@
     </row>
     <row r="29" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>297</v>
+        <v>126</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>298</v>
+        <v>127</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>299</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>53</v>
@@ -4274,7 +4290,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>57</v>
@@ -4288,7 +4304,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>61</v>
@@ -4302,7 +4318,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>68</v>
@@ -4316,142 +4332,142 @@
     </row>
     <row r="34" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -4501,226 +4517,226 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -4741,7 +4757,7 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4775,198 +4791,198 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JSON backend answer parsing was provided!
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" state="visible" r:id="rId2"/>
@@ -41,7 +41,7 @@
     <t xml:space="preserve">ru</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_LOG_IN</t>
+    <t xml:space="preserve">-CPHX_LOG_IN-</t>
   </si>
   <si>
     <t xml:space="preserve">LOGIN</t>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">ЛОГИН</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_LOGIN_INPUT</t>
+    <t xml:space="preserve">-CPHX_LOGIN_INPUT-</t>
   </si>
   <si>
     <t xml:space="preserve">ENTER LOGIN</t>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">ВВЕДИТЕ ЛОГИН</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_PASS_INPUT</t>
+    <t xml:space="preserve">-CPHX_PASS_INPUT-</t>
   </si>
   <si>
     <t xml:space="preserve">ENTER PASSWORD</t>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">ВВЕДИТЕ ПАРОЛЬ</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_LOGIN_BTN</t>
+    <t xml:space="preserve">-CPHX_LOGIN_BTN-</t>
   </si>
   <si>
     <t xml:space="preserve">LOG IN</t>
@@ -89,7 +89,7 @@
     <t xml:space="preserve">ВОЙТИ</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_OLIMPIC_SYSTEM</t>
+    <t xml:space="preserve">-CPHX_OLIMPIC_SYSTEM-</t>
   </si>
   <si>
     <t xml:space="preserve">Olimpic</t>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">Олимпийская</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_CIRCLE_SYSTEM</t>
+    <t xml:space="preserve">-CPHX_CIRCLE_SYSTEM-</t>
   </si>
   <si>
     <t xml:space="preserve">Circle</t>
@@ -113,7 +113,7 @@
     <t xml:space="preserve">Круговая</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_MALE_SEX</t>
+    <t xml:space="preserve">-CPHX_MALE_SEX-</t>
   </si>
   <si>
     <t xml:space="preserve">Male</t>
@@ -125,7 +125,7 @@
     <t xml:space="preserve">Мужской</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_FEMALE_SEX</t>
+    <t xml:space="preserve">-CPHX_FEMALE_SEX-</t>
   </si>
   <si>
     <t xml:space="preserve">Female</t>
@@ -137,7 +137,7 @@
     <t xml:space="preserve">Женский</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_NA</t>
+    <t xml:space="preserve">-CPHX_NA-</t>
   </si>
   <si>
     <t xml:space="preserve">Not applicable</t>
@@ -149,7 +149,7 @@
     <t xml:space="preserve">Не применяется</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_HUMAN_NAME</t>
+    <t xml:space="preserve">-CPHX_HUMAN_NAME-</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -161,7 +161,7 @@
     <t xml:space="preserve">Имя</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_HUMAN_SURNAME</t>
+    <t xml:space="preserve">-CPHX_HUMAN_SURNAME-</t>
   </si>
   <si>
     <t xml:space="preserve">Surname</t>
@@ -173,7 +173,7 @@
     <t xml:space="preserve">Фамилия</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_HUMAN_BD</t>
+    <t xml:space="preserve">-CPHX_HUMAN_BD-</t>
   </si>
   <si>
     <t xml:space="preserve">Birth date</t>
@@ -185,7 +185,7 @@
     <t xml:space="preserve">Дата рождения</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_HUMAN_WEIGHT</t>
+    <t xml:space="preserve">-CPHX_HUMAN_WEIGHT-</t>
   </si>
   <si>
     <t xml:space="preserve">Weight</t>
@@ -197,7 +197,7 @@
     <t xml:space="preserve">Вес</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_HUMAN_SEX</t>
+    <t xml:space="preserve">-CPHX_HUMAN_SEX-</t>
   </si>
   <si>
     <t xml:space="preserve">Sex</t>
@@ -209,7 +209,7 @@
     <t xml:space="preserve">Пол</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_HUMAN_TEAM</t>
+    <t xml:space="preserve">-CPHX_HUMAN_TEAM-</t>
   </si>
   <si>
     <t xml:space="preserve">Team</t>
@@ -218,7 +218,7 @@
     <t xml:space="preserve">Команда</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_HUMAN_REGION</t>
+    <t xml:space="preserve">-CPHX_HUMAN_REGION-</t>
   </si>
   <si>
     <t xml:space="preserve">Region</t>
@@ -230,7 +230,7 @@
     <t xml:space="preserve">Регион</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_QUALIFICATION</t>
+    <t xml:space="preserve">-CPHX_QUALIFICATION-</t>
   </si>
   <si>
     <t xml:space="preserve">Qualification</t>
@@ -242,7 +242,7 @@
     <t xml:space="preserve">Квалификация</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_NOT_HUMAN_NAME</t>
+    <t xml:space="preserve">-CPHX_NOT_HUMAN_NAME-</t>
   </si>
   <si>
     <t xml:space="preserve">Назва</t>
@@ -251,13 +251,13 @@
     <t xml:space="preserve">Название</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_ID</t>
+    <t xml:space="preserve">-CPHX_ID-</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_QUALS</t>
+    <t xml:space="preserve">-CPHX_QUALS-</t>
   </si>
   <si>
     <t xml:space="preserve">Qualifications</t>
@@ -269,7 +269,7 @@
     <t xml:space="preserve">Квалификации</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_YES</t>
+    <t xml:space="preserve">-CPHX_YES-</t>
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
@@ -281,7 +281,7 @@
     <t xml:space="preserve">Да</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_NO</t>
+    <t xml:space="preserve">-CPHX_NO-</t>
   </si>
   <si>
     <t xml:space="preserve">No</t>
@@ -293,10 +293,10 @@
     <t xml:space="preserve">Нет</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_TEAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPHX_EMAIL</t>
+    <t xml:space="preserve">-CPHX_TEAM-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-CPHX_EMAIL-</t>
   </si>
   <si>
     <t xml:space="preserve">Email</t>
@@ -308,7 +308,7 @@
     <t xml:space="preserve">Электронный адрес</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_CHNG_EMAIL_BTN</t>
+    <t xml:space="preserve">-CPHX_CHNG_EMAIL_BTN-</t>
   </si>
   <si>
     <t xml:space="preserve">Change email</t>
@@ -320,7 +320,7 @@
     <t xml:space="preserve">Изменить электронный адрес</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_CHNG_PASS_BTN</t>
+    <t xml:space="preserve">-CPHX_CHNG_PASS_BTN-</t>
   </si>
   <si>
     <t xml:space="preserve">Change password</t>
@@ -332,7 +332,7 @@
     <t xml:space="preserve">Изменить пароль</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_CHNG_EMAIL_POPUP</t>
+    <t xml:space="preserve">-CPHX_CHNG_EMAIL_POPUP-</t>
   </si>
   <si>
     <t xml:space="preserve">CHANGE EMAIL</t>
@@ -344,7 +344,7 @@
     <t xml:space="preserve">СМЕНА АДРЕСА</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_NEW_EMAIL</t>
+    <t xml:space="preserve">-CPHX_NEW_EMAIL-</t>
   </si>
   <si>
     <t xml:space="preserve">ENTER NEW EMAIL</t>
@@ -356,7 +356,7 @@
     <t xml:space="preserve">ВВЕДИТЕ НОВЫЙ АДРЕС</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_CHNG_PASS_POPUP</t>
+    <t xml:space="preserve">-CPHX_CHNG_PASS_POPUP-</t>
   </si>
   <si>
     <t xml:space="preserve">CHANGE PASSWORD</t>
@@ -368,7 +368,7 @@
     <t xml:space="preserve">СМЕНА ПАРОЛЯ</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_OLD_PASS</t>
+    <t xml:space="preserve">-CPHX_OLD_PASS-</t>
   </si>
   <si>
     <t xml:space="preserve">ENTER OLD PASSWORD</t>
@@ -380,7 +380,7 @@
     <t xml:space="preserve">ВВЕДИТЕ СТАРЫЙ ПАРОЛЬ</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_NEW_PASS</t>
+    <t xml:space="preserve">-CPHX_NEW_PASS-</t>
   </si>
   <si>
     <t xml:space="preserve">ENTER NEW PASSWORD</t>
@@ -392,7 +392,7 @@
     <t xml:space="preserve">ВВЕДИТЕ НОВЫЙ ПАРОЛЬ</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_NEW_PASS_AGAIN</t>
+    <t xml:space="preserve">-CPHX_NEW_PASS_AGAIN-</t>
   </si>
   <si>
     <t xml:space="preserve">ENTER NEW PASSWORD AGAIN</t>
@@ -404,7 +404,7 @@
     <t xml:space="preserve">ВВЕДИТЕ НОВЫЙ ПАРОЛЬ СНОВА</t>
   </si>
   <si>
-    <t xml:space="preserve">CPHX_HUMAN_AGE</t>
+    <t xml:space="preserve">-CPHX_HUMAN_AGE-</t>
   </si>
   <si>
     <t xml:space="preserve">Age</t>
@@ -440,7 +440,7 @@
     <t xml:space="preserve">Выйти</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_COMP_TAB</t>
+    <t xml:space="preserve">-PHX_COMP_TAB-</t>
   </si>
   <si>
     <t xml:space="preserve">Competitions</t>
@@ -452,7 +452,7 @@
     <t xml:space="preserve">Соревнования</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_SPORTS_TAB</t>
+    <t xml:space="preserve">-PHX_SPORTS_TAB-</t>
   </si>
   <si>
     <t xml:space="preserve">Sportsmen</t>
@@ -464,7 +464,7 @@
     <t xml:space="preserve">Спортсмены</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_INFO_TAB</t>
+    <t xml:space="preserve">-PHX_INFO_TAB-</t>
   </si>
   <si>
     <t xml:space="preserve">Information</t>
@@ -476,7 +476,7 @@
     <t xml:space="preserve">Информация</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ADD_COMP</t>
+    <t xml:space="preserve">-PHX_ADD_COMP-</t>
   </si>
   <si>
     <t xml:space="preserve">Create competition</t>
@@ -488,7 +488,7 @@
     <t xml:space="preserve">Создать соревнование</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_SPORTS</t>
+    <t xml:space="preserve">-PHX_SPORTS-</t>
   </si>
   <si>
     <t xml:space="preserve">SPORTSMEN</t>
@@ -500,7 +500,7 @@
     <t xml:space="preserve">СПОРТСМЕНЫ</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_DP_INFO</t>
+    <t xml:space="preserve">-PHX_DP_INFO-</t>
   </si>
   <si>
     <t xml:space="preserve">Department Info</t>
@@ -512,7 +512,7 @@
     <t xml:space="preserve">Информация о департаменте</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_VALUE</t>
+    <t xml:space="preserve">-PHX_VALUE-</t>
   </si>
   <si>
     <t xml:space="preserve">Qualification value</t>
@@ -524,7 +524,7 @@
     <t xml:space="preserve">Значение квалификации</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_NAME</t>
+    <t xml:space="preserve">-PHX_NAME-</t>
   </si>
   <si>
     <t xml:space="preserve">Qualification name</t>
@@ -536,7 +536,7 @@
     <t xml:space="preserve">Название квалификации</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_DISCIPLINES</t>
+    <t xml:space="preserve">-PHX_DISCIPLINES-</t>
   </si>
   <si>
     <t xml:space="preserve">Disciplines</t>
@@ -548,7 +548,7 @@
     <t xml:space="preserve">Дисциплины</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_DIS_NAME</t>
+    <t xml:space="preserve">-PHX_DIS_NAME-</t>
   </si>
   <si>
     <t xml:space="preserve">Discipline name</t>
@@ -560,7 +560,7 @@
     <t xml:space="preserve">Название дисциплины</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_CREATE_SPORTS</t>
+    <t xml:space="preserve">-PHX_CREATE_SPORTS-</t>
   </si>
   <si>
     <t xml:space="preserve">Sportsman creation</t>
@@ -572,7 +572,7 @@
     <t xml:space="preserve">Создание спортсмена</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_SP_TRAINER</t>
+    <t xml:space="preserve">-PHX_SP_TRAINER-</t>
   </si>
   <si>
     <t xml:space="preserve">Trainer</t>
@@ -584,7 +584,7 @@
     <t xml:space="preserve">Тренер</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_SP_ADD_ONE_MORE</t>
+    <t xml:space="preserve">-PHX_SP_ADD_ONE_MORE-</t>
   </si>
   <si>
     <t xml:space="preserve">Create one more</t>
@@ -596,7 +596,7 @@
     <t xml:space="preserve">Создать еще одного</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_COMP_DESC</t>
+    <t xml:space="preserve">-PHX_COMP_DESC-</t>
   </si>
   <si>
     <t xml:space="preserve">Competition description</t>
@@ -608,7 +608,7 @@
     <t xml:space="preserve">Описание</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_COMP_START</t>
+    <t xml:space="preserve">-PHX_COMP_START-</t>
   </si>
   <si>
     <t xml:space="preserve">Start date</t>
@@ -620,7 +620,7 @@
     <t xml:space="preserve">Дата начала</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_COMP_END</t>
+    <t xml:space="preserve">-PHX_COMP_END-</t>
   </si>
   <si>
     <t xml:space="preserve">End date</t>
@@ -632,10 +632,10 @@
     <t xml:space="preserve">Дата окончания</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_COMP_CREATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_CREATE_BTN</t>
+    <t xml:space="preserve">-PHX_COMP_CREATE-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_CREATE_BTN-</t>
   </si>
   <si>
     <t xml:space="preserve">Create</t>
@@ -647,7 +647,7 @@
     <t xml:space="preserve">Создать</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_TRAINERS_TAB</t>
+    <t xml:space="preserve">-PHX_TRAINERS_TAB-</t>
   </si>
   <si>
     <t xml:space="preserve">Trainers</t>
@@ -659,7 +659,7 @@
     <t xml:space="preserve">Тренеры</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_TRAINERS</t>
+    <t xml:space="preserve">-PHX_TRAINERS-</t>
   </si>
   <si>
     <t xml:space="preserve">TRAINERS</t>
@@ -671,7 +671,7 @@
     <t xml:space="preserve">ТРЕНЕРЫ</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_CREATE_TRAINER</t>
+    <t xml:space="preserve">-PHX_CREATE_TRAINER-</t>
   </si>
   <si>
     <t xml:space="preserve">Trainer creation</t>
@@ -683,10 +683,10 @@
     <t xml:space="preserve">Создание тренера</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_TEAM_TAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_TRAINER_INFO</t>
+    <t xml:space="preserve">-PHX_TEAM_TAB-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_TRAINER_INFO-</t>
   </si>
   <si>
     <t xml:space="preserve">Trainer information</t>
@@ -698,7 +698,7 @@
     <t xml:space="preserve">Информация про тренера</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_DEL_BTN</t>
+    <t xml:space="preserve">-PHX_DEL_BTN-</t>
   </si>
   <si>
     <t xml:space="preserve">DELETE</t>
@@ -722,7 +722,7 @@
     <t xml:space="preserve">Тенер</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_CHANGE_PHOTO</t>
+    <t xml:space="preserve">-PHX_CHANGE_PHOTO-</t>
   </si>
   <si>
     <t xml:space="preserve">Load new photo</t>
@@ -734,7 +734,7 @@
     <t xml:space="preserve">Загрузить новое фото</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_STAT_TAB</t>
+    <t xml:space="preserve">-PHX_STAT_TAB-</t>
   </si>
   <si>
     <t xml:space="preserve">Statistics</t>
@@ -743,7 +743,7 @@
     <t xml:space="preserve">Статистики</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_SPORT_INFO</t>
+    <t xml:space="preserve">-PHX_SPORT_INFO-</t>
   </si>
   <si>
     <t xml:space="preserve">Sportsman information</t>
@@ -755,31 +755,31 @@
     <t xml:space="preserve">Информация о спортсмене</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_INFO_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_SURNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_SEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_BD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_WEIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_QUAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_TEAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_APPLY_BTN</t>
+    <t xml:space="preserve">-PHX_INFO_ID-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_SURNAME-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_NAME-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_SEX-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_BD-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_WEIGHT-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_QUAL-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_TEAM-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_APPLY_BTN-</t>
   </si>
   <si>
     <t xml:space="preserve">Apply</t>
@@ -791,7 +791,7 @@
     <t xml:space="preserve">Применить</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_COMP_RES</t>
+    <t xml:space="preserve">-PHX_COMP_RES-</t>
   </si>
   <si>
     <t xml:space="preserve">Result</t>
@@ -800,7 +800,7 @@
     <t xml:space="preserve">Результат</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_GROUPS_NUM</t>
+    <t xml:space="preserve">-PHX_GROUPS_NUM-</t>
   </si>
   <si>
     <t xml:space="preserve">Groups</t>
@@ -812,7 +812,7 @@
     <t xml:space="preserve">Группы</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_PAIRS_NUM</t>
+    <t xml:space="preserve">-PHX_PAIRS_NUM-</t>
   </si>
   <si>
     <t xml:space="preserve">Pairs</t>
@@ -824,7 +824,7 @@
     <t xml:space="preserve">Пары</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_WINS_NUM</t>
+    <t xml:space="preserve">-PHX_WINS_NUM-</t>
   </si>
   <si>
     <t xml:space="preserve">Wins</t>
@@ -836,7 +836,7 @@
     <t xml:space="preserve">Победы</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_SCORE</t>
+    <t xml:space="preserve">-PHX_SCORE-</t>
   </si>
   <si>
     <t xml:space="preserve">Score</t>
@@ -848,10 +848,10 @@
     <t xml:space="preserve">Счет</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_DISC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_ADMIT</t>
+    <t xml:space="preserve">-PHX_DISC-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_ADMIT-</t>
   </si>
   <si>
     <t xml:space="preserve">Admittion</t>
@@ -860,7 +860,7 @@
     <t xml:space="preserve">Допуск</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_PLACE</t>
+    <t xml:space="preserve">-PHX_PLACE-</t>
   </si>
   <si>
     <t xml:space="preserve">Place</t>
@@ -881,16 +881,16 @@
     <t xml:space="preserve">Дисциплина</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_TBL_PAIRS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_PAIR_NUM</t>
+    <t xml:space="preserve">-PHX_TBL_PAIRS-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_PAIR_NUM-</t>
   </si>
   <si>
     <t xml:space="preserve">№</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_PAIR_LIST</t>
+    <t xml:space="preserve">-PHX_PAIR_LIST-</t>
   </si>
   <si>
     <t xml:space="preserve">Arena</t>
@@ -899,7 +899,7 @@
     <t xml:space="preserve">Арена</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_PAIR_TIME</t>
+    <t xml:space="preserve">-PHX_PAIR_TIME-</t>
   </si>
   <si>
     <t xml:space="preserve">Time</t>
@@ -911,19 +911,19 @@
     <t xml:space="preserve">Время</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_PAIR_RES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_TRAINER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_REGION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_GROUPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_PAIRS_LISTS</t>
+    <t xml:space="preserve">-PHX_PAIR_RES-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_TRAINER-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_REGION-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_GROUPS-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_PAIRS_LISTS-</t>
   </si>
   <si>
     <t xml:space="preserve">Arenas</t>
@@ -935,10 +935,10 @@
     <t xml:space="preserve">Арены</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_INFORM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_SORT_BTN</t>
+    <t xml:space="preserve">-PHX_INFORM-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_SORT_BTN-</t>
   </si>
   <si>
     <t xml:space="preserve">Update groups composition</t>
@@ -950,7 +950,7 @@
     <t xml:space="preserve">Обновить состав групп</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ADD_GROUP_BTN</t>
+    <t xml:space="preserve">-PHX_ADD_GROUP_BTN-</t>
   </si>
   <si>
     <t xml:space="preserve">Create group</t>
@@ -962,7 +962,7 @@
     <t xml:space="preserve">Создать группу</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_GROUP_UPDATE_BTN</t>
+    <t xml:space="preserve">-PHX_GROUP_UPDATE_BTN-</t>
   </si>
   <si>
     <t xml:space="preserve">Update pairs </t>
@@ -974,7 +974,7 @@
     <t xml:space="preserve">Обновить пары</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_SPORT_REG_BTN</t>
+    <t xml:space="preserve">-PHX_SPORT_REG_BTN-</t>
   </si>
   <si>
     <t xml:space="preserve">Sportsmen registration</t>
@@ -986,37 +986,37 @@
     <t xml:space="preserve">Регистрация спортсменов</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_TBL_SPORTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_SPORT_SURNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_SPORT_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_SPORT_AGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_SPORT_WEIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_SPORT_SEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_SPORT_TEAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_SPORT_QUAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_SPORT_ADMIT</t>
+    <t xml:space="preserve">-PHX_TBL_SPORTS-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_SPORT_SURNAME-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_SPORT_NAME-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_SPORT_AGE-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_SPORT_WEIGHT-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_SPORT_SEX-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_SPORT_TEAM-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_SPORT_QUAL-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_SPORT_ADMIT-</t>
   </si>
   <si>
     <t xml:space="preserve">Admitton</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_SPORT_GR_NUM</t>
+    <t xml:space="preserve">-PHX_SPORT_GR_NUM-</t>
   </si>
   <si>
     <t xml:space="preserve">Groups number</t>
@@ -1028,28 +1028,28 @@
     <t xml:space="preserve">Количество групп</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_TBL_GROUPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_GROUP_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_GROUP_AGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_GROUP_SEX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_GROUP_DISC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_GROUP_WEIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_GROUP_QUAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_GROUP_SP_NUM</t>
+    <t xml:space="preserve">-PHX_TBL_GROUPS-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_GROUP_NAME-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_GROUP_AGE-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_GROUP_SEX-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_GROUP_DISC-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_GROUP_WEIGHT-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_GROUP_QUAL-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_GROUP_SP_NUM-</t>
   </si>
   <si>
     <t xml:space="preserve">Sportsmen number</t>
@@ -1061,7 +1061,7 @@
     <t xml:space="preserve">Количество спортсменов</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ADD_PAIRS_LIST</t>
+    <t xml:space="preserve">-PHX_ADD_PAIRS_LIST-</t>
   </si>
   <si>
     <t xml:space="preserve">Create arena</t>
@@ -1073,22 +1073,22 @@
     <t xml:space="preserve">Создать арену</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_INFO_HEAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_DESC</t>
+    <t xml:space="preserve">-PHX_INFO_HEAD-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_DESC-</t>
   </si>
   <si>
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_INFO_START</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_END</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_SPORTS_ADD</t>
+    <t xml:space="preserve">-PHX_INFO_START-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_END-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_SPORTS_ADD-</t>
   </si>
   <si>
     <t xml:space="preserve">Sportsmen adding</t>
@@ -1109,7 +1109,7 @@
     <t xml:space="preserve">Добавить спортсменов</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ADD_GROUPS</t>
+    <t xml:space="preserve">-PHX_ADD_GROUPS-</t>
   </si>
   <si>
     <t xml:space="preserve">Group creation</t>
@@ -1121,7 +1121,7 @@
     <t xml:space="preserve">Создание группы</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_GROUP_SYSTEM</t>
+    <t xml:space="preserve">-PHX_GROUP_SYSTEM-</t>
   </si>
   <si>
     <t xml:space="preserve">System</t>
@@ -1130,7 +1130,7 @@
     <t xml:space="preserve">Система</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_GROUP_MIN_AGE</t>
+    <t xml:space="preserve">-PHX_GROUP_MIN_AGE-</t>
   </si>
   <si>
     <t xml:space="preserve">Minimal age</t>
@@ -1142,7 +1142,7 @@
     <t xml:space="preserve">Минимальный возраст</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_GROUP_MAX_AGE</t>
+    <t xml:space="preserve">-PHX_GROUP_MAX_AGE-</t>
   </si>
   <si>
     <t xml:space="preserve">Maximal age</t>
@@ -1154,7 +1154,7 @@
     <t xml:space="preserve">Максимальный возраст</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_GROUP_MIN_WEIGHT</t>
+    <t xml:space="preserve">-PHX_GROUP_MIN_WEIGHT-</t>
   </si>
   <si>
     <t xml:space="preserve">Minimal weight</t>
@@ -1166,7 +1166,7 @@
     <t xml:space="preserve">Минимальный вес</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_GROUP_MAX_WEIGHT</t>
+    <t xml:space="preserve">-PHX_GROUP_MAX_WEIGHT-</t>
   </si>
   <si>
     <t xml:space="preserve">Maximal weight</t>
@@ -1178,7 +1178,7 @@
     <t xml:space="preserve">Максимальный вес</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_GROUP_MIN_QUAL</t>
+    <t xml:space="preserve">-PHX_GROUP_MIN_QUAL-</t>
   </si>
   <si>
     <t xml:space="preserve">Minimal qualification</t>
@@ -1190,7 +1190,7 @@
     <t xml:space="preserve">Минимальная квалификация</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_GROUP_MAX_QUAL</t>
+    <t xml:space="preserve">-PHX_GROUP_MAX_QUAL-</t>
   </si>
   <si>
     <t xml:space="preserve">Maximal qualification</t>
@@ -1202,10 +1202,10 @@
     <t xml:space="preserve">Максимальная квалификация</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_GROUP_CREATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_DELETE_COMPETITION</t>
+    <t xml:space="preserve">-PHX_GROUP_CREATE-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_DELETE_COMPETITION-</t>
   </si>
   <si>
     <t xml:space="preserve">DELETE COMPETITION</t>
@@ -1217,7 +1217,7 @@
     <t xml:space="preserve">УДАЛИТЬ СОРЕВНОВАНИЕ</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ARENA_PAIRS_NUM</t>
+    <t xml:space="preserve">-PHX_ARENA_PAIRS_NUM-</t>
   </si>
   <si>
     <t xml:space="preserve">Pairs number</t>
@@ -1232,10 +1232,10 @@
     <t xml:space="preserve">Group info</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_PAIRS_TAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_GRID_TAB</t>
+    <t xml:space="preserve">-PHX_PAIRS_TAB-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_GRID_TAB-</t>
   </si>
   <si>
     <t xml:space="preserve">Grid</t>
@@ -1247,31 +1247,31 @@
     <t xml:space="preserve">Сетка</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_INFO_SYSTEM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_DISCIPLINE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_LOW_AGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_TOP_AGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_LOW_WEIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_TOP_WEIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_LOW_QUAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_INFO_TOP_QUAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_FORMULAS</t>
+    <t xml:space="preserve">-PHX_INFO_SYSTEM-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_DISCIPLINE-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_LOW_AGE-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_TOP_AGE-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_LOW_WEIGHT-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_TOP_WEIGHT-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_LOW_QUAL-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_INFO_TOP_QUAL-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_FORMULAS-</t>
   </si>
   <si>
     <t xml:space="preserve">Formulas</t>
@@ -1283,7 +1283,7 @@
     <t xml:space="preserve">Формулы</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_PREPARATION</t>
+    <t xml:space="preserve">-PHX_PREPARATION-</t>
   </si>
   <si>
     <t xml:space="preserve">Preparation</t>
@@ -1295,7 +1295,7 @@
     <t xml:space="preserve">Подготовка</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ROUNDS_NUM</t>
+    <t xml:space="preserve">-PHX_ROUNDS_NUM-</t>
   </si>
   <si>
     <t xml:space="preserve">Rounds number</t>
@@ -1307,7 +1307,7 @@
     <t xml:space="preserve">Количество раундов</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ROUND</t>
+    <t xml:space="preserve">-PHX_ROUND-</t>
   </si>
   <si>
     <t xml:space="preserve">Round</t>
@@ -1316,7 +1316,7 @@
     <t xml:space="preserve">Раунд</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_REST</t>
+    <t xml:space="preserve">-PHX_REST-</t>
   </si>
   <si>
     <t xml:space="preserve">Rest</t>
@@ -1328,7 +1328,7 @@
     <t xml:space="preserve">Отдых</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_HOLD</t>
+    <t xml:space="preserve">-PHX_HOLD-</t>
   </si>
   <si>
     <t xml:space="preserve">Delay</t>
@@ -1340,7 +1340,7 @@
     <t xml:space="preserve">Задержка</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_FINAL_MIN</t>
+    <t xml:space="preserve">-PHX_FINAL_MIN-</t>
   </si>
   <si>
     <t xml:space="preserve">Minimal final part</t>
@@ -1352,7 +1352,7 @@
     <t xml:space="preserve">Минимальная финальная часть</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_FINAL_MAX</t>
+    <t xml:space="preserve">-PHX_FINAL_MAX-</t>
   </si>
   <si>
     <t xml:space="preserve">Maximal final part</t>
@@ -1364,13 +1364,13 @@
     <t xml:space="preserve">Максимальная финальная часть</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_DELETE_BTN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_PAIRS_LIST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_PAIR_FINAL</t>
+    <t xml:space="preserve">-PHX_DELETE_BTN-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_PAIRS_LIST-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_PAIR_FINAL-</t>
   </si>
   <si>
     <t xml:space="preserve">Final part</t>
@@ -1382,7 +1382,7 @@
     <t xml:space="preserve">Финальная часть</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_PAIR_RED</t>
+    <t xml:space="preserve">-PHX_PAIR_RED-</t>
   </si>
   <si>
     <t xml:space="preserve">Red corner</t>
@@ -1394,7 +1394,7 @@
     <t xml:space="preserve">Красный угол</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_PAIR_BLUE</t>
+    <t xml:space="preserve">-PHX_PAIR_BLUE-</t>
   </si>
   <si>
     <t xml:space="preserve">Blue corner</t>
@@ -1406,7 +1406,7 @@
     <t xml:space="preserve">Синий угол</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_PAIR_WIN</t>
+    <t xml:space="preserve">-PHX_PAIR_WIN-</t>
   </si>
   <si>
     <t xml:space="preserve">Winner</t>
@@ -1418,16 +1418,16 @@
     <t xml:space="preserve">Победитель</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ADD_SPORTS</t>
+    <t xml:space="preserve">-PHX_ADD_SPORTS-</t>
   </si>
   <si>
     <t xml:space="preserve">Додати спортсменів </t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_PAGE_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_PLACE_NAME</t>
+    <t xml:space="preserve">-PHX_PAGE_NAME-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_PLACE_NAME-</t>
   </si>
   <si>
     <t xml:space="preserve">Arena name</t>
@@ -1439,7 +1439,7 @@
     <t xml:space="preserve">Название арены</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_AUTOSORT_TAB</t>
+    <t xml:space="preserve">-PHX_AUTOSORT_TAB-</t>
   </si>
   <si>
     <t xml:space="preserve">Automatic sorting</t>
@@ -1451,7 +1451,7 @@
     <t xml:space="preserve">Автоматическая сортировка</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_MANUAL_TAB</t>
+    <t xml:space="preserve">-PHX_MANUAL_TAB-</t>
   </si>
   <si>
     <t xml:space="preserve">Manual sorting</t>
@@ -1463,7 +1463,7 @@
     <t xml:space="preserve">Ручная сортировка</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ACTIVE_GROUPS_LIST</t>
+    <t xml:space="preserve">-PHX_ACTIVE_GROUPS_LIST-</t>
   </si>
   <si>
     <t xml:space="preserve">Selected groups</t>
@@ -1475,7 +1475,7 @@
     <t xml:space="preserve">Выбранные группы</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_UNACTIVE_GROUPS_LIST</t>
+    <t xml:space="preserve">-PHX_UNACTIVE_GROUPS_LIST-</t>
   </si>
   <si>
     <t xml:space="preserve">Groups list</t>
@@ -1487,7 +1487,7 @@
     <t xml:space="preserve">Список групп</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_DISTANCE</t>
+    <t xml:space="preserve">-PHX_DISTANCE-</t>
   </si>
   <si>
     <t xml:space="preserve">One member pairs distance</t>
@@ -1499,22 +1499,22 @@
     <t xml:space="preserve">Расстояние между парами одного участника</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_AGE_MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_AGE_MAX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_WEIGHT_MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_WEIGHT_MAX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_QUALIFICATION_MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_QUALIFICATION_MAX</t>
+    <t xml:space="preserve">-PHX_AGE_MIN-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_AGE_MAX-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_WEIGHT_MIN-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_WEIGHT_MAX-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_QUALIFICATION_MIN-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_QUALIFICATION_MAX-</t>
   </si>
   <si>
     <t xml:space="preserve">CREATE</t>
@@ -1526,7 +1526,7 @@
     <t xml:space="preserve">СОЗДАТЬ</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ACTIVE_PAIRS_LIST</t>
+    <t xml:space="preserve">-PHX_ACTIVE_PAIRS_LIST-</t>
   </si>
   <si>
     <t xml:space="preserve">Selected pairs</t>
@@ -1538,7 +1538,7 @@
     <t xml:space="preserve">Выбранные пары</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_UNACTIVE_PAIRS_LIST</t>
+    <t xml:space="preserve">-PHX_UNACTIVE_PAIRS_LIST-</t>
   </si>
   <si>
     <t xml:space="preserve">Unattached pairs</t>
@@ -1550,7 +1550,7 @@
     <t xml:space="preserve">Непривязанные пары</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_SCHEDULE_NAME</t>
+    <t xml:space="preserve">-PHX_SCHEDULE_NAME-</t>
   </si>
   <si>
     <t xml:space="preserve">SCHEDULE</t>
@@ -1562,7 +1562,7 @@
     <t xml:space="preserve">РАСПИСАНИЕ</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_SCHEDULE_START</t>
+    <t xml:space="preserve">-PHX_SCHEDULE_START-</t>
   </si>
   <si>
     <t xml:space="preserve">Work start</t>
@@ -1574,7 +1574,7 @@
     <t xml:space="preserve">Начало работы</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_SCHEDULE_END</t>
+    <t xml:space="preserve">-PHX_SCHEDULE_END-</t>
   </si>
   <si>
     <t xml:space="preserve">Work end</t>
@@ -1592,7 +1592,7 @@
     <t xml:space="preserve">Список пар</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_SETTINGS</t>
+    <t xml:space="preserve">-PHX_SETTINGS-</t>
   </si>
   <si>
     <t xml:space="preserve">Settings</t>
@@ -1604,16 +1604,16 @@
     <t xml:space="preserve">Настройки</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_TIME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_RED_SPORTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_BLUE_SPORTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_GROUP</t>
+    <t xml:space="preserve">-PHX_TIME-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_RED_SPORTS-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_BLUE_SPORTS-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_GROUP-</t>
   </si>
   <si>
     <t xml:space="preserve">Group</t>
@@ -1625,10 +1625,10 @@
     <t xml:space="preserve">Группа</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_WINNER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHX_RED_SCORE</t>
+    <t xml:space="preserve">-PHX_WINNER-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_RED_SCORE-</t>
   </si>
   <si>
     <t xml:space="preserve">Red score</t>
@@ -1640,7 +1640,7 @@
     <t xml:space="preserve">Красный счёт</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_BLUE_SCORE</t>
+    <t xml:space="preserve">-PHX_BLUE_SCORE-</t>
   </si>
   <si>
     <t xml:space="preserve">Blue score</t>
@@ -1652,7 +1652,7 @@
     <t xml:space="preserve">Синий счёт</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_PAIR_WINNER</t>
+    <t xml:space="preserve">-PHX_PAIR_WINNER-</t>
   </si>
   <si>
     <t xml:space="preserve">Winner of pair</t>
@@ -1664,7 +1664,7 @@
     <t xml:space="preserve">Победитель пары</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_REFRESH_LIST</t>
+    <t xml:space="preserve">-PHX_REFRESH_LIST-</t>
   </si>
   <si>
     <t xml:space="preserve">Refresh the list</t>
@@ -1676,7 +1676,7 @@
     <t xml:space="preserve">Обновить список</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_START_LIST</t>
+    <t xml:space="preserve">-PHX_START_LIST-</t>
   </si>
   <si>
     <t xml:space="preserve">Start list</t>
@@ -1688,7 +1688,7 @@
     <t xml:space="preserve">Старт списка</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_DELETE_ARENA</t>
+    <t xml:space="preserve">-PHX_DELETE_ARENA-</t>
   </si>
   <si>
     <t xml:space="preserve">Delete arena</t>
@@ -1709,7 +1709,7 @@
     <t xml:space="preserve">НАЗВАНИЕ АРЕНЫ</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ATTACHED_GROUPS_TBL</t>
+    <t xml:space="preserve">-PHX_ATTACHED_GROUPS_TBL-</t>
   </si>
   <si>
     <t xml:space="preserve">GROUPS</t>
@@ -1730,7 +1730,7 @@
     <t xml:space="preserve">ПРИМЕНИТЬ</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ADD_PAIRS_TO_LIST</t>
+    <t xml:space="preserve">-PHX_ADD_PAIRS_TO_LIST-</t>
   </si>
   <si>
     <t xml:space="preserve">NEW PAIRS ADDING</t>
@@ -1742,7 +1742,7 @@
     <t xml:space="preserve">ДОБАВЛЕНИЕ НОВЫХ ПАР</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ADD_PAIRS_BTN</t>
+    <t xml:space="preserve">-PHX_ADD_PAIRS_BTN-</t>
   </si>
   <si>
     <t xml:space="preserve">ADD</t>
@@ -1754,7 +1754,7 @@
     <t xml:space="preserve">ДОБАВИТЬ</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ADD_GROUPS_TO_LIST</t>
+    <t xml:space="preserve">-PHX_ADD_GROUPS_TO_LIST-</t>
   </si>
   <si>
     <t xml:space="preserve">NEW GROUPS ADDING</t>
@@ -1766,7 +1766,7 @@
     <t xml:space="preserve">ДОБАВЛЕНИЕ НОВЫХ ГРУПП</t>
   </si>
   <si>
-    <t xml:space="preserve">PHX_ADD_GROUPS_BTN</t>
+    <t xml:space="preserve">-PHX_ADD_GROUPS_BTN-</t>
   </si>
 </sst>
 </file>
@@ -1776,7 +1776,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1798,6 +1798,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1842,7 +1848,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1853,6 +1859,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1875,7 +1889,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2788,7 +2802,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3477,7 +3491,7 @@
   </sheetPr>
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -4164,10 +4178,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4195,7 +4209,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>145</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>400</v>
@@ -4222,7 +4236,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="3" t="s">
         <v>401</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -4262,6 +4276,7 @@
       <c r="D6" s="0" t="s">
         <v>148</v>
       </c>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -4781,6 +4796,8 @@
         <v>359</v>
       </c>
     </row>
+    <row r="1048562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5138,8 +5155,8 @@
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Searching in sportsmen table on competition page was added. Clickable admittion in tables was provided.
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="580">
   <si>
     <t xml:space="preserve">origin</t>
   </si>
@@ -1776,7 +1776,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1798,12 +1798,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1848,7 +1842,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1859,14 +1853,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1886,10 +1872,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2403,6 +2389,34 @@
       </c>
       <c r="D36" s="0" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -4180,8 +4194,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4209,7 +4223,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>145</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>400</v>
@@ -4236,7 +4250,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>401</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -4276,7 +4290,7 @@
       <c r="D6" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -5155,7 +5169,7 @@
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Searchin row styles were updated
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="586">
   <si>
     <t xml:space="preserve">origin</t>
   </si>
@@ -440,6 +440,18 @@
     <t xml:space="preserve">Выйти</t>
   </si>
   <si>
+    <t xml:space="preserve">-CPHX_TABLE_SEARCHING-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пошук</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Поиск</t>
+  </si>
+  <si>
     <t xml:space="preserve">-PHX_COMP_TAB-</t>
   </si>
   <si>
@@ -1425,6 +1437,12 @@
   </si>
   <si>
     <t xml:space="preserve">-PHX_PAGE_NAME-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Створення арени</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Создание арены</t>
   </si>
   <si>
     <t xml:space="preserve">-PHX_PLACE_NAME-</t>
@@ -1872,10 +1890,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
+      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2417,6 +2435,20 @@
       </c>
       <c r="D38" s="0" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2467,310 +2499,310 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2842,21 +2874,21 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>61</v>
@@ -2870,114 +2902,114 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3027,49 +3059,49 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>75</v>
@@ -3083,7 +3115,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>45</v>
@@ -3097,7 +3129,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>41</v>
@@ -3111,7 +3143,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>57</v>
@@ -3125,7 +3157,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>49</v>
@@ -3139,7 +3171,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>53</v>
@@ -3153,7 +3185,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>68</v>
@@ -3167,7 +3199,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>61</v>
@@ -3181,287 +3213,287 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>64</v>
@@ -3475,16 +3507,16 @@
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -3534,133 +3566,133 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>45</v>
@@ -3674,7 +3706,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>41</v>
@@ -3688,7 +3720,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>126</v>
@@ -3702,7 +3734,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>53</v>
@@ -3716,7 +3748,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>57</v>
@@ -3730,7 +3762,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>61</v>
@@ -3744,7 +3776,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>68</v>
@@ -3758,49 +3790,49 @@
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>41</v>
@@ -3814,7 +3846,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>126</v>
@@ -3828,7 +3860,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>57</v>
@@ -3842,21 +3874,21 @@
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>53</v>
@@ -3870,7 +3902,7 @@
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>68</v>
@@ -3884,49 +3916,49 @@
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>75</v>
@@ -3940,7 +3972,7 @@
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>41</v>
@@ -3954,226 +3986,226 @@
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -4223,78 +4255,78 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>41</v>
@@ -4308,35 +4340,35 @@
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>57</v>
@@ -4350,231 +4382,231 @@
     </row>
     <row r="11" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>45</v>
@@ -4588,7 +4620,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>41</v>
@@ -4602,7 +4634,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>126</v>
@@ -4616,7 +4648,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>53</v>
@@ -4630,7 +4662,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>57</v>
@@ -4644,7 +4676,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>61</v>
@@ -4658,7 +4690,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>68</v>
@@ -4672,142 +4704,142 @@
     </row>
     <row r="34" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="1048562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4828,10 +4860,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4859,298 +4891,299 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>346</v>
+        <v>470</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>347</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>518</v>
-      </c>
-    </row>
+        <v>524</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5198,464 +5231,464 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>534</v>
+        <v>540</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>539</v>
+        <v>545</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>540</v>
+        <v>546</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>541</v>
+        <v>547</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>542</v>
+        <v>548</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>547</v>
+        <v>553</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>548</v>
+        <v>554</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>551</v>
+        <v>557</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>552</v>
+        <v>558</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>554</v>
+        <v>560</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>555</v>
+        <v>561</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>556</v>
+        <v>562</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>557</v>
+        <v>563</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>559</v>
+        <v>565</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>561</v>
+        <v>567</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>565</v>
+        <v>571</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>566</v>
+        <v>572</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>568</v>
+        <v>574</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>569</v>
+        <v>575</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>570</v>
+        <v>576</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>572</v>
+        <v>578</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>574</v>
+        <v>580</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>575</v>
+        <v>581</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>576</v>
+        <v>582</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>577</v>
+        <v>583</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>578</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>579</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>572</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>573</v>
-      </c>
       <c r="D34" s="0" t="s">
-        <v>574</v>
+        <v>580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common tables styles were provided
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="593">
   <si>
     <t xml:space="preserve">origin</t>
   </si>
@@ -113,6 +113,18 @@
     <t xml:space="preserve">Круговая</t>
   </si>
   <si>
+    <t xml:space="preserve">-CPHX_MALE_SHORT-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ч</t>
+  </si>
+  <si>
+    <t xml:space="preserve">М</t>
+  </si>
+  <si>
     <t xml:space="preserve">-CPHX_MALE_SEX-</t>
   </si>
   <si>
@@ -125,6 +137,15 @@
     <t xml:space="preserve">Мужской</t>
   </si>
   <si>
+    <t xml:space="preserve">-CPHX_FEMALE_SHORT-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ж</t>
+  </si>
+  <si>
     <t xml:space="preserve">-CPHX_FEMALE_SEX-</t>
   </si>
   <si>
@@ -1031,13 +1052,13 @@
     <t xml:space="preserve">-PHX_SPORT_GR_NUM-</t>
   </si>
   <si>
-    <t xml:space="preserve">Groups number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кількість груп</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Количество групп</t>
+    <t xml:space="preserve">Group&lt;/br&gt;number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">К-ть&lt;/br&gt;груп</t>
+  </si>
+  <si>
+    <t xml:space="preserve">К-во&lt;/br&gt;групп</t>
   </si>
   <si>
     <t xml:space="preserve">-PHX_TBL_GROUPS-</t>
@@ -1794,7 +1815,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1816,6 +1837,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1860,7 +1887,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1871,6 +1898,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1890,10 +1921,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E19:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2003,7 +2034,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>28</v>
       </c>
@@ -2031,8 +2062,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -2042,88 +2073,88 @@
         <v>38</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="C12" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="C14" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="C15" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="C16" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>62</v>
@@ -2144,30 +2175,30 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="B19" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="0" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2175,280 +2206,308 @@
       <c r="A20" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>75</v>
+      <c r="C20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="C22" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="1" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>62</v>
+      <c r="C24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="C25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>93</v>
+      <c r="A26" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="D26" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="C27" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="D27" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="C28" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="D28" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="0" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="B29" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="C29" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="1" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="C30" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="D30" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="D30" s="0" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="B31" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D31" s="0" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="C32" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="D32" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="D33" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="0" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="B34" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="C34" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="D34" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="D34" s="0" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="C35" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="D35" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="D35" s="0" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="B36" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="C36" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="D36" s="0" t="s">
         <v>135</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
       <c r="D38" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="B39" s="0" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>140</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2470,7 +2529,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="E19:E20 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2499,310 +2558,310 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2848,7 +2907,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E19:E20 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2874,142 +2933,142 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3031,7 +3090,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+      <selection pane="topLeft" activeCell="C37" activeCellId="1" sqref="E19:E20 C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3059,464 +3118,464 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3537,8 +3596,8 @@
   </sheetPr>
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="1" sqref="E19:E20 D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3566,646 +3625,646 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>334</v>
+        <v>340</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>341</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -4227,7 +4286,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="1" sqref="E19:E20 D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4255,591 +4314,591 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>426</v>
+        <v>433</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>431</v>
+        <v>438</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
     </row>
     <row r="1048562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4863,7 +4922,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="1" sqref="E19:E20 F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4891,296 +4950,296 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>475</v>
+        <v>482</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5203,7 +5262,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+      <selection pane="topLeft" activeCell="E39" activeCellId="1" sqref="E19:E20 E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5231,464 +5290,464 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>431</v>
+        <v>438</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>532</v>
+        <v>539</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>534</v>
+        <v>541</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>535</v>
+        <v>542</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>536</v>
+        <v>543</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>538</v>
+        <v>545</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>546</v>
+        <v>553</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>548</v>
+        <v>555</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>549</v>
+        <v>556</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>550</v>
+        <v>557</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>551</v>
+        <v>558</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>552</v>
+        <v>559</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>553</v>
+        <v>560</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>554</v>
+        <v>561</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>555</v>
+        <v>562</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>557</v>
+        <v>564</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>558</v>
+        <v>565</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>563</v>
+        <v>570</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>567</v>
+        <v>574</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>570</v>
+        <v>577</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>574</v>
+        <v>581</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>576</v>
+        <v>583</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>577</v>
+        <v>584</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>578</v>
+        <v>585</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>580</v>
+        <v>587</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>581</v>
+        <v>588</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>583</v>
+        <v>590</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>592</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>585</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>578</v>
-      </c>
       <c r="C34" s="0" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>580</v>
+        <v>587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All tables were updated
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="617">
   <si>
     <t xml:space="preserve">origin</t>
   </si>
@@ -533,6 +533,18 @@
     <t xml:space="preserve">СПОРТСМЕНЫ</t>
   </si>
   <si>
+    <t xml:space="preserve">-PHX_SPORTS_CREATE-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create sportsman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Створити спортсмена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Создать спортсмена</t>
+  </si>
+  <si>
     <t xml:space="preserve">-PHX_DP_INFO-</t>
   </si>
   <si>
@@ -704,6 +716,18 @@
     <t xml:space="preserve">ТРЕНЕРЫ</t>
   </si>
   <si>
+    <t xml:space="preserve">-PHX_TRAINER_CREATE-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create trainer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Створити тренера</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Создать тренера</t>
+  </si>
+  <si>
     <t xml:space="preserve">-PHX_CREATE_TRAINER-</t>
   </si>
   <si>
@@ -767,6 +791,18 @@
     <t xml:space="preserve">Загрузить новое фото</t>
   </si>
   <si>
+    <t xml:space="preserve">-PHX_SPORT_ADD_BTN-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add sportsman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Додати спортсмена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добавить спортсмена</t>
+  </si>
+  <si>
     <t xml:space="preserve">-PHX_STAT_TAB-</t>
   </si>
   <si>
@@ -1454,7 +1490,43 @@
     <t xml:space="preserve">-PHX_ADD_SPORTS-</t>
   </si>
   <si>
-    <t xml:space="preserve">Додати спортсменів </t>
+    <t xml:space="preserve">Add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Додати </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добавить</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_ADD_SPORTS_BTN-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Додати спортсменів</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_UPDATE_PAIRS-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Оновити</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Обновить</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_TBL_ADD_SPORTS-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD SPORTSMEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ДОДАВАННЯ СПОРТСМЕНІВ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ДОБАВЛЕНИЕ СПОРТСМЕНОВ</t>
   </si>
   <si>
     <t xml:space="preserve">-PHX_PAGE_NAME-</t>
@@ -1815,7 +1887,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1837,12 +1909,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1900,8 +1966,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1923,8 +1989,8 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E19:E20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2526,10 +2592,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="E19:E20 A3"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2626,7 +2692,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>168</v>
       </c>
@@ -2640,8 +2706,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2668,8 +2734,8 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>180</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2682,8 +2748,8 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2766,8 +2832,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>208</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2785,31 +2851,31 @@
         <v>212</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>161</v>
+        <v>213</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>162</v>
+        <v>214</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>163</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>214</v>
+        <v>161</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>215</v>
+        <v>162</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
         <v>217</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2837,35 +2903,61 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2888,6 +2980,8 @@
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2904,10 +2998,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="E19:E20 A2"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2947,7 +3041,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>68</v>
@@ -2961,16 +3055,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2989,86 +3083,100 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -3090,7 +3198,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="1" sqref="E19:E20 C37"/>
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3132,35 +3240,35 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>82</v>
@@ -3174,7 +3282,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>52</v>
@@ -3188,7 +3296,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>48</v>
@@ -3202,7 +3310,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>64</v>
@@ -3216,7 +3324,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>56</v>
@@ -3230,7 +3338,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>60</v>
@@ -3244,7 +3352,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>75</v>
@@ -3258,7 +3366,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>68</v>
@@ -3272,287 +3380,287 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>71</v>
@@ -3566,16 +3674,16 @@
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3597,7 +3705,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="1" sqref="E19:E20 D25"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3639,35 +3747,35 @@
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>311</v>
+        <v>323</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>157</v>
@@ -3681,63 +3789,63 @@
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>323</v>
+        <v>335</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>329</v>
+        <v>341</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>153</v>
@@ -3751,7 +3859,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>52</v>
@@ -3765,7 +3873,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>48</v>
@@ -3779,7 +3887,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>133</v>
@@ -3793,7 +3901,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>60</v>
@@ -3807,7 +3915,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>64</v>
@@ -3821,7 +3929,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>68</v>
@@ -3835,7 +3943,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>337</v>
+        <v>349</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>75</v>
@@ -3849,49 +3957,49 @@
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>340</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>341</v>
+        <v>352</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>342</v>
+        <v>354</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>343</v>
+        <v>355</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>48</v>
@@ -3905,7 +4013,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>133</v>
@@ -3919,7 +4027,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>64</v>
@@ -3933,21 +4041,21 @@
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>60</v>
@@ -3961,7 +4069,7 @@
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>75</v>
@@ -3975,35 +4083,35 @@
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>355</v>
+        <v>367</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>157</v>
@@ -4017,7 +4125,7 @@
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>82</v>
@@ -4031,7 +4139,7 @@
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>48</v>
@@ -4045,226 +4153,226 @@
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>361</v>
+        <v>373</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>362</v>
+        <v>374</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>365</v>
+        <v>377</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>366</v>
+        <v>378</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>367</v>
+        <v>379</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>368</v>
+        <v>380</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>369</v>
+        <v>381</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>372</v>
+        <v>384</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>375</v>
+        <v>387</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>382</v>
+        <v>394</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>386</v>
+        <v>398</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>388</v>
+        <v>400</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>402</v>
+        <v>414</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>403</v>
+        <v>415</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>406</v>
+        <v>418</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>409</v>
+        <v>421</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -4285,8 +4393,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="1" sqref="E19:E20 D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4317,7 +4425,7 @@
         <v>156</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>158</v>
@@ -4342,35 +4450,35 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>412</v>
+        <v>424</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>413</v>
+        <v>425</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>414</v>
+        <v>426</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>415</v>
+        <v>427</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>416</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>157</v>
@@ -4385,7 +4493,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>48</v>
@@ -4399,35 +4507,35 @@
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>418</v>
+        <v>430</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>64</v>
@@ -4441,217 +4549,217 @@
     </row>
     <row r="11" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>419</v>
+        <v>431</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>420</v>
+        <v>432</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>388</v>
+        <v>400</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>422</v>
+        <v>434</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>425</v>
+        <v>437</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>431</v>
+        <v>443</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>432</v>
+        <v>444</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>153</v>
@@ -4665,7 +4773,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>52</v>
@@ -4679,7 +4787,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>48</v>
@@ -4693,7 +4801,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>133</v>
@@ -4707,7 +4815,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>60</v>
@@ -4721,7 +4829,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>64</v>
@@ -4735,7 +4843,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>68</v>
@@ -4749,7 +4857,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>337</v>
+        <v>349</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>75</v>
@@ -4763,142 +4871,184 @@
     </row>
     <row r="34" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>460</v>
+        <v>472</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>461</v>
+        <v>473</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>466</v>
+        <v>478</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>468</v>
+        <v>480</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>470</v>
+        <v>482</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>473</v>
+        <v>485</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>474</v>
+        <v>486</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>368</v>
+        <v>487</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>475</v>
+        <v>488</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>370</v>
+        <v>489</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="1048562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4922,7 +5072,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="1" sqref="E19:E20 F8"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4950,296 +5100,296 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>476</v>
+        <v>500</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>477</v>
+        <v>501</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>478</v>
+        <v>502</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>479</v>
+        <v>503</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>480</v>
+        <v>504</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>481</v>
+        <v>505</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>482</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>483</v>
+        <v>507</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>484</v>
+        <v>508</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>485</v>
+        <v>509</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>486</v>
+        <v>510</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>487</v>
+        <v>511</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>488</v>
+        <v>512</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>489</v>
+        <v>513</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>490</v>
+        <v>514</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>491</v>
+        <v>515</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>492</v>
+        <v>516</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>493</v>
+        <v>517</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>494</v>
+        <v>518</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>495</v>
+        <v>519</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>496</v>
+        <v>520</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>497</v>
+        <v>521</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>498</v>
+        <v>522</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>499</v>
+        <v>523</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>500</v>
+        <v>524</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>501</v>
+        <v>525</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>502</v>
+        <v>526</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>503</v>
+        <v>527</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>504</v>
+        <v>528</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>505</v>
+        <v>529</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>388</v>
+        <v>400</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>506</v>
+        <v>530</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>507</v>
+        <v>531</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>508</v>
+        <v>532</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>509</v>
+        <v>533</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>510</v>
+        <v>534</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>511</v>
+        <v>535</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>512</v>
+        <v>536</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>513</v>
+        <v>537</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>514</v>
+        <v>538</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>515</v>
+        <v>539</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>516</v>
+        <v>540</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>517</v>
+        <v>541</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>518</v>
+        <v>542</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>519</v>
+        <v>543</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>520</v>
+        <v>544</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>521</v>
+        <v>545</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>522</v>
+        <v>546</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>523</v>
+        <v>547</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>524</v>
+        <v>548</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>525</v>
+        <v>549</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>526</v>
+        <v>550</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>527</v>
+        <v>551</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>528</v>
+        <v>552</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>529</v>
+        <v>553</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>530</v>
+        <v>554</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>531</v>
+        <v>555</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5262,7 +5412,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="1" sqref="E19:E20 E39"/>
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5290,464 +5440,464 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>532</v>
+        <v>556</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>533</v>
+        <v>557</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>533</v>
+        <v>557</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>534</v>
+        <v>558</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>535</v>
+        <v>559</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>536</v>
+        <v>560</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>537</v>
+        <v>561</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>538</v>
+        <v>562</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>539</v>
+        <v>563</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>540</v>
+        <v>564</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>468</v>
+        <v>480</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>541</v>
+        <v>565</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>542</v>
+        <v>566</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>543</v>
+        <v>567</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>544</v>
+        <v>568</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>545</v>
+        <v>569</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>473</v>
+        <v>485</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>546</v>
+        <v>570</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>547</v>
+        <v>571</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>548</v>
+        <v>572</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>549</v>
+        <v>573</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>550</v>
+        <v>574</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>551</v>
+        <v>575</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>552</v>
+        <v>576</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>553</v>
+        <v>577</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>554</v>
+        <v>578</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>555</v>
+        <v>579</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>556</v>
+        <v>580</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>557</v>
+        <v>581</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>558</v>
+        <v>582</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>559</v>
+        <v>583</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>560</v>
+        <v>584</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>561</v>
+        <v>585</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>562</v>
+        <v>586</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>563</v>
+        <v>587</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>564</v>
+        <v>588</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>565</v>
+        <v>589</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>566</v>
+        <v>590</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>567</v>
+        <v>591</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>568</v>
+        <v>592</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>569</v>
+        <v>593</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>479</v>
+        <v>503</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>570</v>
+        <v>594</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>571</v>
+        <v>595</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>572</v>
+        <v>596</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>520</v>
+        <v>544</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>521</v>
+        <v>545</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>522</v>
+        <v>546</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>523</v>
+        <v>547</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>524</v>
+        <v>548</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>525</v>
+        <v>549</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>526</v>
+        <v>550</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>527</v>
+        <v>551</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>528</v>
+        <v>552</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>529</v>
+        <v>553</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>530</v>
+        <v>554</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>531</v>
+        <v>555</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>573</v>
+        <v>597</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>574</v>
+        <v>598</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>575</v>
+        <v>599</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>576</v>
+        <v>600</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>499</v>
+        <v>523</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>500</v>
+        <v>524</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>501</v>
+        <v>525</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>502</v>
+        <v>526</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>503</v>
+        <v>527</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>504</v>
+        <v>528</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>505</v>
+        <v>529</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>388</v>
+        <v>400</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>506</v>
+        <v>530</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>507</v>
+        <v>531</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>508</v>
+        <v>532</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>577</v>
+        <v>601</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>578</v>
+        <v>602</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>579</v>
+        <v>603</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>580</v>
+        <v>604</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>581</v>
+        <v>605</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>582</v>
+        <v>606</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>583</v>
+        <v>607</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>584</v>
+        <v>608</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>585</v>
+        <v>609</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>586</v>
+        <v>610</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>587</v>
+        <v>611</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>588</v>
+        <v>612</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>589</v>
+        <v>613</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>590</v>
+        <v>614</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>591</v>
+        <v>615</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>592</v>
+        <v>616</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>585</v>
+        <v>609</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>586</v>
+        <v>610</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>587</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Registration of clients was provided. Form works on department page yet
</commit_message>
<xml_diff>
--- a/translator/dictionary.xlsx
+++ b/translator/dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="637">
   <si>
     <t xml:space="preserve">origin</t>
   </si>
@@ -738,6 +738,66 @@
   </si>
   <si>
     <t xml:space="preserve">Создание тренера</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_CREATE_MEMBER-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Реєстрація</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Регистрация</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_STATUS-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Статус</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_STATUS_TRAINER-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_STATUS_JUDGE-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Суддя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Судья</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_STATUS_ADMIN-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Адміністратор</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Администратор</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-PHX_CONFIRM REG_BTN-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Зареєструватись</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Зарегестрироваться</t>
   </si>
   <si>
     <t xml:space="preserve">-PHX_TEAM_TAB-</t>
@@ -2592,10 +2652,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2958,12 +3018,90 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3041,7 +3179,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>68</v>
@@ -3055,16 +3193,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3083,16 +3221,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3100,13 +3238,13 @@
         <v>192</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3117,10 +3255,10 @@
         <v>197</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3139,16 +3277,16 @@
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3167,16 +3305,16 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -3240,35 +3378,35 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>82</v>
@@ -3282,7 +3420,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>52</v>
@@ -3296,7 +3434,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>48</v>
@@ -3310,7 +3448,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>64</v>
@@ -3324,7 +3462,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>56</v>
@@ -3338,7 +3476,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>60</v>
@@ -3352,7 +3490,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>75</v>
@@ -3366,7 +3504,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>272</v>
+        <v>292</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>68</v>
@@ -3380,105 +3518,105 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>185</v>
@@ -3492,161 +3630,161 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>307</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>197</v>
@@ -3660,7 +3798,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>71</v>
@@ -3674,16 +3812,16 @@
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3747,35 +3885,35 @@
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>157</v>
@@ -3789,63 +3927,63 @@
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>326</v>
+        <v>346</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>327</v>
+        <v>347</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>329</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>331</v>
+        <v>351</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>333</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>336</v>
+        <v>356</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>337</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>338</v>
+        <v>358</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>341</v>
+        <v>361</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>153</v>
@@ -3859,7 +3997,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>343</v>
+        <v>363</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>52</v>
@@ -3873,7 +4011,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>344</v>
+        <v>364</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>48</v>
@@ -3887,7 +4025,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>133</v>
@@ -3901,7 +4039,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>60</v>
@@ -3915,7 +4053,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>64</v>
@@ -3929,7 +4067,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>348</v>
+        <v>368</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>68</v>
@@ -3943,7 +4081,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>75</v>
@@ -3957,49 +4095,49 @@
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>351</v>
+        <v>371</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>352</v>
+        <v>372</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>353</v>
+        <v>373</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>354</v>
+        <v>374</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>283</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>357</v>
+        <v>377</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>48</v>
@@ -4013,7 +4151,7 @@
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>358</v>
+        <v>378</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>133</v>
@@ -4027,7 +4165,7 @@
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>359</v>
+        <v>379</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>64</v>
@@ -4041,21 +4179,21 @@
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>360</v>
+        <v>380</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>361</v>
+        <v>381</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>60</v>
@@ -4069,7 +4207,7 @@
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>362</v>
+        <v>382</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>75</v>
@@ -4083,35 +4221,35 @@
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>363</v>
+        <v>383</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>364</v>
+        <v>384</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>366</v>
+        <v>386</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>367</v>
+        <v>387</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>368</v>
+        <v>388</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>369</v>
+        <v>389</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>370</v>
+        <v>390</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>371</v>
+        <v>391</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>157</v>
@@ -4125,7 +4263,7 @@
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>82</v>
@@ -4139,7 +4277,7 @@
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>48</v>
@@ -4153,10 +4291,10 @@
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>372</v>
+        <v>392</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>206</v>
@@ -4167,7 +4305,7 @@
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>374</v>
+        <v>394</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>209</v>
@@ -4181,7 +4319,7 @@
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>375</v>
+        <v>395</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>213</v>
@@ -4195,184 +4333,184 @@
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>376</v>
+        <v>396</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>377</v>
+        <v>397</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>378</v>
+        <v>398</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>379</v>
+        <v>399</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>376</v>
+        <v>396</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>382</v>
+        <v>402</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>383</v>
+        <v>403</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>384</v>
+        <v>404</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>385</v>
+        <v>405</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>386</v>
+        <v>406</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>387</v>
+        <v>407</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>388</v>
+        <v>408</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>389</v>
+        <v>409</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>389</v>
+        <v>409</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>390</v>
+        <v>410</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>391</v>
+        <v>411</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>392</v>
+        <v>412</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>393</v>
+        <v>413</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>394</v>
+        <v>414</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>395</v>
+        <v>415</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>396</v>
+        <v>416</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>397</v>
+        <v>417</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>398</v>
+        <v>418</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>399</v>
+        <v>419</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>401</v>
+        <v>421</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>402</v>
+        <v>422</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>403</v>
+        <v>423</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>404</v>
+        <v>424</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>405</v>
+        <v>425</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>406</v>
+        <v>426</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>407</v>
+        <v>427</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>408</v>
+        <v>428</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>409</v>
+        <v>429</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>410</v>
+        <v>430</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>411</v>
+        <v>431</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>412</v>
+        <v>432</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>413</v>
+        <v>433</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>414</v>
+        <v>434</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>331</v>
+        <v>351</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>333</v>
+        <v>353</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>415</v>
+        <v>435</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>416</v>
+        <v>436</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>417</v>
+        <v>437</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>418</v>
+        <v>438</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>419</v>
+        <v>439</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>420</v>
+        <v>440</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>421</v>
+        <v>441</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>422</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -4393,8 +4531,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4425,7 +4563,7 @@
         <v>156</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>423</v>
+        <v>443</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>158</v>
@@ -4450,35 +4588,35 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>424</v>
+        <v>444</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>425</v>
+        <v>445</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>426</v>
+        <v>446</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>427</v>
+        <v>447</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>428</v>
+        <v>448</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>371</v>
+        <v>391</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>157</v>
@@ -4493,7 +4631,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>48</v>
@@ -4507,35 +4645,35 @@
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>429</v>
+        <v>449</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>388</v>
+        <v>408</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>389</v>
+        <v>409</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>389</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>430</v>
+        <v>450</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>64</v>
@@ -4549,217 +4687,217 @@
     </row>
     <row r="11" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>431</v>
+        <v>451</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>391</v>
+        <v>411</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>392</v>
+        <v>412</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>393</v>
+        <v>413</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>432</v>
+        <v>452</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>395</v>
+        <v>415</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>396</v>
+        <v>416</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>397</v>
+        <v>417</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>433</v>
+        <v>453</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>399</v>
+        <v>419</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>401</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>434</v>
+        <v>454</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>395</v>
+        <v>415</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>404</v>
+        <v>424</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>405</v>
+        <v>425</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>435</v>
+        <v>455</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>407</v>
+        <v>427</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>408</v>
+        <v>428</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>409</v>
+        <v>429</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>436</v>
+        <v>456</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>411</v>
+        <v>431</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>412</v>
+        <v>432</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>413</v>
+        <v>433</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>437</v>
+        <v>457</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>438</v>
+        <v>458</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>439</v>
+        <v>459</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>440</v>
+        <v>460</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>441</v>
+        <v>461</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>442</v>
+        <v>462</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>443</v>
+        <v>463</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>444</v>
+        <v>464</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>445</v>
+        <v>465</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>446</v>
+        <v>466</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>447</v>
+        <v>467</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>448</v>
+        <v>468</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>449</v>
+        <v>469</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>450</v>
+        <v>470</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>451</v>
+        <v>471</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>451</v>
+        <v>471</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>452</v>
+        <v>472</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>453</v>
+        <v>473</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>454</v>
+        <v>474</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>455</v>
+        <v>475</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>456</v>
+        <v>476</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>457</v>
+        <v>477</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>458</v>
+        <v>478</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>459</v>
+        <v>479</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>460</v>
+        <v>480</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>461</v>
+        <v>481</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>463</v>
+        <v>483</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>464</v>
+        <v>484</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>465</v>
+        <v>485</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>466</v>
+        <v>486</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>467</v>
+        <v>487</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>468</v>
+        <v>488</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>153</v>
@@ -4773,7 +4911,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>343</v>
+        <v>363</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>52</v>
@@ -4787,7 +4925,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>344</v>
+        <v>364</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>48</v>
@@ -4801,7 +4939,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>133</v>
@@ -4815,7 +4953,7 @@
     </row>
     <row r="30" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>60</v>
@@ -4829,7 +4967,7 @@
     </row>
     <row r="31" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>64</v>
@@ -4843,7 +4981,7 @@
     </row>
     <row r="32" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>348</v>
+        <v>368</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>68</v>
@@ -4857,7 +4995,7 @@
     </row>
     <row r="33" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>75</v>
@@ -4871,184 +5009,184 @@
     </row>
     <row r="34" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>307</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>287</v>
+        <v>307</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>469</v>
+        <v>489</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>470</v>
+        <v>490</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>471</v>
+        <v>491</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>472</v>
+        <v>492</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>473</v>
+        <v>493</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>474</v>
+        <v>494</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>475</v>
+        <v>495</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>476</v>
+        <v>496</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>477</v>
+        <v>497</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>478</v>
+        <v>498</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>479</v>
+        <v>499</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>480</v>
+        <v>500</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>481</v>
+        <v>501</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>482</v>
+        <v>502</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>484</v>
+        <v>504</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>485</v>
+        <v>505</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>486</v>
+        <v>506</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>487</v>
+        <v>507</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>488</v>
+        <v>508</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>489</v>
+        <v>509</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>490</v>
+        <v>510</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>491</v>
+        <v>511</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>382</v>
+        <v>402</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>492</v>
+        <v>512</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>493</v>
+        <v>513</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>494</v>
+        <v>514</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>495</v>
+        <v>515</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>496</v>
+        <v>516</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>497</v>
+        <v>517</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>498</v>
+        <v>518</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>499</v>
+        <v>519</v>
       </c>
     </row>
     <row r="1048562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5100,296 +5238,296 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>500</v>
+        <v>520</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>368</v>
+        <v>388</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>501</v>
+        <v>521</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>502</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>503</v>
+        <v>523</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>504</v>
+        <v>524</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>505</v>
+        <v>525</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>506</v>
+        <v>526</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>507</v>
+        <v>527</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>508</v>
+        <v>528</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>509</v>
+        <v>529</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>510</v>
+        <v>530</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>511</v>
+        <v>531</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>512</v>
+        <v>532</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>513</v>
+        <v>533</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>514</v>
+        <v>534</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>515</v>
+        <v>535</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>516</v>
+        <v>536</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>517</v>
+        <v>537</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>518</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>519</v>
+        <v>539</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>520</v>
+        <v>540</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>521</v>
+        <v>541</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>522</v>
+        <v>542</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>523</v>
+        <v>543</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>524</v>
+        <v>544</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>525</v>
+        <v>545</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>526</v>
+        <v>546</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>527</v>
+        <v>547</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>391</v>
+        <v>411</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>392</v>
+        <v>412</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>393</v>
+        <v>413</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>528</v>
+        <v>548</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>395</v>
+        <v>415</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>396</v>
+        <v>416</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>397</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>529</v>
+        <v>549</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>399</v>
+        <v>419</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>401</v>
+        <v>421</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>530</v>
+        <v>550</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>403</v>
+        <v>423</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>404</v>
+        <v>424</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>405</v>
+        <v>425</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>460</v>
+        <v>480</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>461</v>
+        <v>481</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>463</v>
+        <v>483</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>464</v>
+        <v>484</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>465</v>
+        <v>485</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>466</v>
+        <v>486</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>467</v>
+        <v>487</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>531</v>
+        <v>551</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>407</v>
+        <v>427</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>408</v>
+        <v>428</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>409</v>
+        <v>429</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>411</v>
+        <v>431</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>412</v>
+        <v>432</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>413</v>
+        <v>433</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>533</v>
+        <v>553</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>534</v>
+        <v>554</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>535</v>
+        <v>555</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>536</v>
+        <v>556</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>537</v>
+        <v>557</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>538</v>
+        <v>558</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>539</v>
+        <v>559</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>540</v>
+        <v>560</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>541</v>
+        <v>561</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>542</v>
+        <v>562</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>543</v>
+        <v>563</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>544</v>
+        <v>564</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>545</v>
+        <v>565</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>546</v>
+        <v>566</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>547</v>
+        <v>567</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>548</v>
+        <v>568</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>549</v>
+        <v>569</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>551</v>
+        <v>571</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>552</v>
+        <v>572</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>553</v>
+        <v>573</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>554</v>
+        <v>574</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>555</v>
+        <v>575</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5440,464 +5578,464 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>469</v>
+        <v>489</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>556</v>
+        <v>576</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>557</v>
+        <v>577</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>557</v>
+        <v>577</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>558</v>
+        <v>578</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>559</v>
+        <v>579</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>560</v>
+        <v>580</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>561</v>
+        <v>581</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>449</v>
+        <v>469</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>450</v>
+        <v>470</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>451</v>
+        <v>471</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>451</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>562</v>
+        <v>582</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>563</v>
+        <v>583</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>475</v>
+        <v>495</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>476</v>
+        <v>496</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>477</v>
+        <v>497</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>564</v>
+        <v>584</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>479</v>
+        <v>499</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>480</v>
+        <v>500</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>481</v>
+        <v>501</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>565</v>
+        <v>585</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>566</v>
+        <v>586</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>567</v>
+        <v>587</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>568</v>
+        <v>588</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>569</v>
+        <v>589</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>484</v>
+        <v>504</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>485</v>
+        <v>505</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>570</v>
+        <v>590</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>571</v>
+        <v>591</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>572</v>
+        <v>592</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>573</v>
+        <v>593</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>574</v>
+        <v>594</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>575</v>
+        <v>595</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>576</v>
+        <v>596</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>577</v>
+        <v>597</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>578</v>
+        <v>598</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>579</v>
+        <v>599</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>580</v>
+        <v>600</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>581</v>
+        <v>601</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>582</v>
+        <v>602</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>583</v>
+        <v>603</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>584</v>
+        <v>604</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>585</v>
+        <v>605</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>586</v>
+        <v>606</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>587</v>
+        <v>607</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>588</v>
+        <v>608</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>589</v>
+        <v>609</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>590</v>
+        <v>610</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>591</v>
+        <v>611</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>592</v>
+        <v>612</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>593</v>
+        <v>613</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>503</v>
+        <v>523</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>594</v>
+        <v>614</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>595</v>
+        <v>615</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>596</v>
+        <v>616</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>544</v>
+        <v>564</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>545</v>
+        <v>565</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>546</v>
+        <v>566</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>547</v>
+        <v>567</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>548</v>
+        <v>568</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>549</v>
+        <v>569</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>551</v>
+        <v>571</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>552</v>
+        <v>572</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>553</v>
+        <v>573</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>554</v>
+        <v>574</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>555</v>
+        <v>575</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>597</v>
+        <v>617</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>598</v>
+        <v>618</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>599</v>
+        <v>619</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>600</v>
+        <v>620</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>523</v>
+        <v>543</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>524</v>
+        <v>544</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>525</v>
+        <v>545</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>526</v>
+        <v>546</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>527</v>
+        <v>547</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>391</v>
+        <v>411</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>392</v>
+        <v>412</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>393</v>
+        <v>413</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>528</v>
+        <v>548</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>395</v>
+        <v>415</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>396</v>
+        <v>416</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>397</v>
+        <v>417</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>529</v>
+        <v>549</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>399</v>
+        <v>419</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>401</v>
+        <v>421</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>530</v>
+        <v>550</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>403</v>
+        <v>423</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>404</v>
+        <v>424</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>405</v>
+        <v>425</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>460</v>
+        <v>480</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>461</v>
+        <v>481</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>462</v>
+        <v>482</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>463</v>
+        <v>483</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>464</v>
+        <v>484</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>465</v>
+        <v>485</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>466</v>
+        <v>486</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>467</v>
+        <v>487</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>531</v>
+        <v>551</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>407</v>
+        <v>427</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>408</v>
+        <v>428</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>409</v>
+        <v>429</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>411</v>
+        <v>431</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>412</v>
+        <v>432</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>413</v>
+        <v>433</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>601</v>
+        <v>621</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>602</v>
+        <v>622</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>603</v>
+        <v>623</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>604</v>
+        <v>624</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>605</v>
+        <v>625</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>606</v>
+        <v>626</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>607</v>
+        <v>627</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>608</v>
+        <v>628</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>609</v>
+        <v>629</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>610</v>
+        <v>630</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>611</v>
+        <v>631</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>612</v>
+        <v>632</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>613</v>
+        <v>633</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>614</v>
+        <v>634</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>615</v>
+        <v>635</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>616</v>
+        <v>636</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>609</v>
+        <v>629</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>610</v>
+        <v>630</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>611</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>